<commit_message>
updating RTM and UT_IT_Plans
</commit_message>
<xml_diff>
--- a/RTM/RTM_CDR.xlsx
+++ b/RTM/RTM_CDR.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miKzggqRmdBW2lOFYGMCeuNZW4iCw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjNEUga4RtWQyGng5vHf9e9pj5AnQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Req</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Client(),Server()</t>
   </si>
   <si>
-    <t>TC_01,TC_02</t>
+    <t>STC_01,RTC_01</t>
   </si>
   <si>
     <t>CONN_01,CONN_02</t>
@@ -51,10 +51,10 @@
     <t>PSI_02</t>
   </si>
   <si>
-    <t>setDetails(),registerDetails(),getDetails(),showMenu(0)</t>
-  </si>
-  <si>
-    <t>TC_03,TC_04</t>
+    <t>setDetails(),getDetails(),showMenu(0)</t>
+  </si>
+  <si>
+    <t>STC_02,STC_03,STC_04</t>
   </si>
   <si>
     <t>REG_03,REG_04</t>
@@ -66,7 +66,7 @@
     <t>verifyLoginCreds(),userExists()</t>
   </si>
   <si>
-    <t>TC_05,TC_06,TC_07,TC_08,TC_09.TC_10</t>
+    <t>STC_05,RTC_02,RTC_03,RTC_04,RTC_05,RTC_06,RTC_07</t>
   </si>
   <si>
     <t>LOGIN_05,LOGIN_06</t>
@@ -81,7 +81,7 @@
     <t>User</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>RTC_06,RTC_07</t>
   </si>
   <si>
     <t>PSI_05</t>
@@ -93,22 +93,28 @@
     <t>showMenu(1)</t>
   </si>
   <si>
+    <t>RTC_08,RTC_09,RTC_10,RTC_11,RTC_12,STC_07,STC_08,STC_09,STC_10,STC_11</t>
+  </si>
+  <si>
     <t>PCDR_01,PCDR_02</t>
   </si>
   <si>
     <t>PSI_06</t>
   </si>
   <si>
-    <t xml:space="preserve"> processCallData()</t>
-  </si>
-  <si>
-    <t>TC_11,TC_12.TC_27,TC_28,TC_29,TC_30,TC_31,TC_32,TC_33,TC_34</t>
+    <t>processCallData(), processAndCreateFile(), processCDR(), mapToFile()</t>
+  </si>
+  <si>
+    <t>STC_12,RTC_13,RTC_14,RTC_15,RTC_16</t>
   </si>
   <si>
     <t>PSI_07</t>
   </si>
   <si>
-    <t>mapToFile()</t>
+    <t>processCDR()</t>
+  </si>
+  <si>
+    <t>STC_13,RTC_17</t>
   </si>
   <si>
     <t>PSI_08</t>
@@ -117,7 +123,7 @@
     <t>4.3.4</t>
   </si>
   <si>
-    <t>processCDR()</t>
+    <t>STC_12,RTC_13,RTC_14,RTC_15,RTC_16,STC_16,RTC_19,RTC_20,RTC_21</t>
   </si>
   <si>
     <t>PSI_09</t>
@@ -126,16 +132,16 @@
     <t>showMenu(2)</t>
   </si>
   <si>
+    <t>STC_17,RTC_22,STC_18,RTC_23</t>
+  </si>
+  <si>
     <t>CB_03</t>
   </si>
   <si>
     <t>PSI_10</t>
   </si>
   <si>
-    <t>searchMSISDN(),sendFile()</t>
-  </si>
-  <si>
-    <t>TC_20,TC_21,TC_22,TC_23</t>
+    <t>processCDR(), mapToFile(), searchMSISDN(), sendFile(),  writeToFile()</t>
   </si>
   <si>
     <t>CB_01,CB_02</t>
@@ -144,7 +150,10 @@
     <t>PSI_11</t>
   </si>
   <si>
-    <t>sendFile(),searchBrandName()</t>
+    <t>processCDR(), mapToFile(), searchBrandName(), sendFile(), writeToFile()</t>
+  </si>
+  <si>
+    <t>STC_16,RTC_19,RTC_20,RTC_21</t>
   </si>
   <si>
     <t>IB_01,IB_02</t>
@@ -156,20 +165,32 @@
     <t>closeServer()</t>
   </si>
   <si>
+    <t>STC_20,RTC_25</t>
+  </si>
+  <si>
     <t>EXIT_01</t>
   </si>
   <si>
     <t>PSI_13</t>
   </si>
   <si>
+    <t>4.3.5</t>
+  </si>
+  <si>
     <t>log()</t>
+  </si>
+  <si>
+    <t>STC_19,RTC_24</t>
+  </si>
+  <si>
+    <t>EXIT_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -192,8 +213,8 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -208,13 +229,18 @@
     </font>
     <font>
       <sz val="11.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -230,7 +256,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,8 +275,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border/>
     <border>
       <left/>
@@ -271,25 +303,39 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -297,25 +343,49 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -534,8 +604,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="18.0"/>
     <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="39.71"/>
-    <col customWidth="1" min="4" max="4" width="25.0"/>
+    <col customWidth="1" min="3" max="3" width="75.71"/>
+    <col customWidth="1" min="4" max="4" width="54.29"/>
     <col customWidth="1" min="5" max="5" width="30.14"/>
     <col customWidth="1" min="6" max="26" width="8.71"/>
   </cols>
@@ -550,7 +620,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -558,292 +628,285 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6"/>
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="E6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" ht="18.0" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="E11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="6"/>
+      <c r="C12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="A13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-    </row>
+      <c r="A21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1"/>
     <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
@@ -1822,7 +1885,6 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>